<commit_message>
Tri des fonctions glmm et suppression des scripts inutilisés
</commit_message>
<xml_diff>
--- a/raw_data/mod_bay.xlsx
+++ b/raw_data/mod_bay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA160D2-E837-44C8-B163-78F7F1026126}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCEDCDC-5BC8-426B-B5D6-9A1DF877C715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{1C948670-4AF4-4636-B722-E5FD7C805F62}"/>
   </bookViews>
@@ -87,10 +87,10 @@
     <t>sig_bay</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>***</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -541,7 +541,7 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -597,7 +597,7 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -625,7 +625,7 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour après midi 10/07
</commit_message>
<xml_diff>
--- a/raw_data/mod_bay.xlsx
+++ b/raw_data/mod_bay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lea.bouchet\Documents\Artif\Artif\liste_rouge_regionale\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCEDCDC-5BC8-426B-B5D6-9A1DF877C715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453B8EFE-CEF7-491E-A700-F3864C97D10E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{1C948670-4AF4-4636-B722-E5FD7C805F62}"/>
   </bookViews>
@@ -90,7 +90,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>***</t>
+    <t>[*]</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>